<commit_message>
Update camp timetable files for cello and flute with new data. Ensure all relevant files are current and reflect the latest schedule changes.
</commit_message>
<xml_diff>
--- a/input/flute-campA-time-table.xlsx
+++ b/input/flute-campA-time-table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lmski\Desktop\Timetable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{033202A3-4953-4F91-91C4-821680318897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B04C26-F64D-402F-A2FF-700D0F68BF72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" activeTab="5" xr2:uid="{4F305ACA-9255-4D6C-9A65-1407DE2CF383}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="56">
   <si>
     <t xml:space="preserve">Time </t>
   </si>
@@ -71,9 +71,6 @@
   </si>
   <si>
     <t>Teacher</t>
-  </si>
-  <si>
-    <t>Workshop</t>
   </si>
   <si>
     <t>Group 6</t>
@@ -195,9 +192,6 @@
 (Room Group Activity)</t>
   </si>
   <si>
-    <t>Welcome</t>
-  </si>
-  <si>
     <t>F2  Private Lesson with Stephane RETY &amp; pianist</t>
   </si>
   <si>
@@ -227,13 +221,26 @@
   <si>
     <t>After Concert Dinner 
 (Pheasant-Jasmine Room, Mandarin Oriental)</t>
+  </si>
+  <si>
+    <t>Welcome
+School Tour
+Fire Drill</t>
+  </si>
+  <si>
+    <t>Yoga Class
+(Room Yoga)</t>
+  </si>
+  <si>
+    <t>Workshop - Warm Up
+(Room Stephane)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -253,20 +260,14 @@
       <family val="2"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -307,6 +308,12 @@
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.89999084444715716"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF1CEEE"/>
+        <bgColor rgb="FFF1CEEE"/>
       </patternFill>
     </fill>
   </fills>
@@ -636,7 +643,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -659,128 +666,149 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -789,66 +817,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -867,24 +835,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -897,9 +847,15 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -912,12 +868,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1255,7 +1209,7 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:G6"/>
+      <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1268,11 +1222,11 @@
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="81" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="81" t="s">
         <v>23</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
@@ -1286,68 +1240,68 @@
       <c r="A3" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="19"/>
+      <c r="B3" s="80" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="4">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="22"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="80"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="4">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="22"/>
+      <c r="B5" s="80"/>
+      <c r="C5" s="80"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="80"/>
+      <c r="F5" s="80"/>
+      <c r="G5" s="80"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="4">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="25"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B6" s="80"/>
+      <c r="C6" s="80"/>
+      <c r="D6" s="80"/>
+      <c r="E6" s="80"/>
+      <c r="F6" s="80"/>
+      <c r="G6" s="80"/>
+    </row>
+    <row r="7" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="15" t="s">
+      <c r="D7" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="23" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1357,7 +1311,7 @@
       </c>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
+      <c r="D8" s="16"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
@@ -1368,7 +1322,7 @@
       </c>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
+      <c r="D9" s="16"/>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
       <c r="G9" s="11"/>
@@ -1379,7 +1333,7 @@
       </c>
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
+      <c r="D10" s="17"/>
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
       <c r="G10" s="12"/>
@@ -1388,22 +1342,22 @@
       <c r="A11" s="4">
         <v>0.5</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="14" t="s">
+      <c r="D11" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="F11" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="14" t="s">
+      <c r="G11" s="10" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1414,7 +1368,7 @@
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
-      <c r="E12" s="15"/>
+      <c r="E12" s="23"/>
       <c r="F12" s="11"/>
       <c r="G12" s="11"/>
     </row>
@@ -1425,7 +1379,7 @@
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
-      <c r="E13" s="15"/>
+      <c r="E13" s="23"/>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
     </row>
@@ -1436,7 +1390,7 @@
       <c r="B14" s="12"/>
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
-      <c r="E14" s="16"/>
+      <c r="E14" s="31"/>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
     </row>
@@ -1444,68 +1398,68 @@
       <c r="A15" s="4">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="32"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="32"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="4">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="33"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="4">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="33"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="34"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="4">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="33"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="4">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="D19" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="E19" s="14" t="s">
+      <c r="D19" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F19" s="14" t="s">
+      <c r="F19" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G19" s="14" t="s">
+      <c r="G19" s="10" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1546,22 +1500,22 @@
       <c r="A23" s="4">
         <v>0.625</v>
       </c>
-      <c r="B23" s="35" t="s">
+      <c r="B23" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E23" s="27" t="s">
+      <c r="D23" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="F23" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="G23" s="14"/>
+      <c r="G23" s="10"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="4">
@@ -1569,9 +1523,9 @@
       </c>
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
       <c r="G24" s="11"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
@@ -1580,9 +1534,9 @@
       </c>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
       <c r="G25" s="11"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
@@ -1591,38 +1545,38 @@
       </c>
       <c r="B26" s="12"/>
       <c r="C26" s="12"/>
-      <c r="D26" s="37"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
       <c r="G26" s="12"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="4">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B27" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" s="39" t="s">
-        <v>22</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="E27" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
+      <c r="B27" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="4">
         <v>0.67708333333333304</v>
       </c>
       <c r="B28" s="11"/>
-      <c r="C28" s="40"/>
-      <c r="D28" s="40"/>
-      <c r="E28" s="28"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="20"/>
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
     </row>
@@ -1631,9 +1585,9 @@
         <v>0.6875</v>
       </c>
       <c r="B29" s="11"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="28"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="20"/>
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
     </row>
@@ -1642,9 +1596,9 @@
         <v>0.69791666666666696</v>
       </c>
       <c r="B30" s="12"/>
-      <c r="C30" s="41"/>
-      <c r="D30" s="41"/>
-      <c r="E30" s="29"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="21"/>
       <c r="F30" s="12"/>
       <c r="G30" s="12"/>
     </row>
@@ -1659,10 +1613,10 @@
       <c r="A32" s="4">
         <v>0.718749999999999</v>
       </c>
-      <c r="B32" s="38" t="s">
+      <c r="B32" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C32" s="38" t="s">
+      <c r="C32" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1715,14 +1669,16 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="G27:G30"/>
-    <mergeCell ref="B32:B38"/>
-    <mergeCell ref="C32:C38"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="C27:C30"/>
-    <mergeCell ref="D27:D30"/>
-    <mergeCell ref="E27:E30"/>
-    <mergeCell ref="F27:F30"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="B3:G6"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="G7:G10"/>
+    <mergeCell ref="F11:F14"/>
+    <mergeCell ref="G11:G14"/>
+    <mergeCell ref="B7:B10"/>
     <mergeCell ref="E23:E26"/>
     <mergeCell ref="F23:F26"/>
     <mergeCell ref="G23:G26"/>
@@ -1739,16 +1695,14 @@
     <mergeCell ref="B23:B26"/>
     <mergeCell ref="C23:C26"/>
     <mergeCell ref="D23:D26"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="B3:G6"/>
-    <mergeCell ref="F7:F10"/>
-    <mergeCell ref="G7:G10"/>
-    <mergeCell ref="F11:F14"/>
-    <mergeCell ref="G11:G14"/>
-    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="G27:G30"/>
+    <mergeCell ref="B32:B38"/>
+    <mergeCell ref="C32:C38"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="D27:D30"/>
+    <mergeCell ref="E27:E30"/>
+    <mergeCell ref="F27:F30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1759,7 +1713,7 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19:C22"/>
+      <selection activeCell="B3" sqref="B3:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1772,11 +1726,11 @@
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="81" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="81" t="s">
         <v>23</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
@@ -1788,68 +1742,68 @@
       <c r="A3" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="19"/>
+      <c r="B3" s="80" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="4">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="22"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="80"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="4">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="22"/>
+      <c r="B5" s="80"/>
+      <c r="C5" s="80"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="80"/>
+      <c r="F5" s="80"/>
+      <c r="G5" s="80"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="4">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="25"/>
+      <c r="B6" s="80"/>
+      <c r="C6" s="80"/>
+      <c r="D6" s="80"/>
+      <c r="E6" s="80"/>
+      <c r="F6" s="80"/>
+      <c r="G6" s="80"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="22" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="42" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="23" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1858,7 +1812,7 @@
         <v>0.46875</v>
       </c>
       <c r="B8" s="11"/>
-      <c r="C8" s="43"/>
+      <c r="C8" s="32"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
@@ -1869,7 +1823,7 @@
         <v>0.47916666666666702</v>
       </c>
       <c r="B9" s="11"/>
-      <c r="C9" s="43"/>
+      <c r="C9" s="32"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
@@ -1880,7 +1834,7 @@
         <v>0.48958333333333298</v>
       </c>
       <c r="B10" s="12"/>
-      <c r="C10" s="44"/>
+      <c r="C10" s="33"/>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
@@ -1890,22 +1844,22 @@
       <c r="A11" s="4">
         <v>0.5</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="45" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" s="14" t="s">
+      <c r="B11" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="F11" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="14" t="s">
+      <c r="G11" s="10" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1914,7 +1868,7 @@
         <v>0.51041666666666696</v>
       </c>
       <c r="B12" s="11"/>
-      <c r="C12" s="43"/>
+      <c r="C12" s="32"/>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
@@ -1925,7 +1879,7 @@
         <v>0.52083333333333304</v>
       </c>
       <c r="B13" s="11"/>
-      <c r="C13" s="43"/>
+      <c r="C13" s="32"/>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
@@ -1936,7 +1890,7 @@
         <v>0.53125</v>
       </c>
       <c r="B14" s="11"/>
-      <c r="C14" s="43"/>
+      <c r="C14" s="32"/>
       <c r="D14" s="11"/>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
@@ -1946,68 +1900,68 @@
       <c r="A15" s="4">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="46" t="s">
+      <c r="B15" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="47"/>
-      <c r="D15" s="47"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="47"/>
-      <c r="G15" s="48"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="36"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="4">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="49"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="50"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="38"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="4">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="49"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="50"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="38"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="4">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="51"/>
-      <c r="C18" s="52"/>
-      <c r="D18" s="52"/>
-      <c r="E18" s="52"/>
-      <c r="F18" s="52"/>
-      <c r="G18" s="53"/>
+      <c r="B18" s="39"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="41"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="4">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="26" t="s">
-        <v>15</v>
+      <c r="B19" s="22" t="s">
+        <v>14</v>
       </c>
       <c r="C19" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="E19" s="15" t="s">
+      <c r="E19" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="F19" s="15" t="s">
+      <c r="F19" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="G19" s="15" t="s">
+      <c r="G19" s="23" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2016,7 +1970,7 @@
         <v>0.59375</v>
       </c>
       <c r="B20" s="11"/>
-      <c r="C20" s="43"/>
+      <c r="C20" s="32"/>
       <c r="D20" s="11"/>
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
@@ -2027,7 +1981,7 @@
         <v>0.60416666666666696</v>
       </c>
       <c r="B21" s="11"/>
-      <c r="C21" s="43"/>
+      <c r="C21" s="32"/>
       <c r="D21" s="11"/>
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
@@ -2038,7 +1992,7 @@
         <v>0.61458333333333304</v>
       </c>
       <c r="B22" s="12"/>
-      <c r="C22" s="44"/>
+      <c r="C22" s="33"/>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
@@ -2048,32 +2002,32 @@
       <c r="A23" s="4">
         <v>0.625</v>
       </c>
-      <c r="B23" s="35" t="s">
+      <c r="B23" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E23" s="27" t="s">
+      <c r="D23" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="F23" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="G23" s="14"/>
+      <c r="G23" s="10"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="4">
         <v>0.63541666666666696</v>
       </c>
       <c r="B24" s="11"/>
-      <c r="C24" s="43"/>
+      <c r="C24" s="32"/>
       <c r="D24" s="11"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
       <c r="G24" s="11"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
@@ -2081,10 +2035,10 @@
         <v>0.64583333333333304</v>
       </c>
       <c r="B25" s="11"/>
-      <c r="C25" s="43"/>
+      <c r="C25" s="32"/>
       <c r="D25" s="11"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
       <c r="G25" s="11"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
@@ -2092,39 +2046,39 @@
         <v>0.65625</v>
       </c>
       <c r="B26" s="12"/>
-      <c r="C26" s="44"/>
+      <c r="C26" s="33"/>
       <c r="D26" s="12"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
       <c r="G26" s="12"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="4">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B27" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" s="39" t="s">
-        <v>22</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="E27" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
+      <c r="B27" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="4">
         <v>0.67708333333333304</v>
       </c>
       <c r="B28" s="11"/>
-      <c r="C28" s="40"/>
+      <c r="C28" s="16"/>
       <c r="D28" s="11"/>
-      <c r="E28" s="28"/>
+      <c r="E28" s="20"/>
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
     </row>
@@ -2133,9 +2087,9 @@
         <v>0.6875</v>
       </c>
       <c r="B29" s="11"/>
-      <c r="C29" s="40"/>
+      <c r="C29" s="16"/>
       <c r="D29" s="11"/>
-      <c r="E29" s="28"/>
+      <c r="E29" s="20"/>
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
     </row>
@@ -2144,9 +2098,9 @@
         <v>0.69791666666666696</v>
       </c>
       <c r="B30" s="12"/>
-      <c r="C30" s="41"/>
+      <c r="C30" s="17"/>
       <c r="D30" s="12"/>
-      <c r="E30" s="29"/>
+      <c r="E30" s="21"/>
       <c r="F30" s="12"/>
       <c r="G30" s="12"/>
     </row>
@@ -2165,10 +2119,10 @@
       <c r="A32" s="4">
         <v>0.718749999999999</v>
       </c>
-      <c r="B32" s="38" t="s">
+      <c r="B32" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C32" s="38" t="s">
+      <c r="C32" s="13" t="s">
         <v>8</v>
       </c>
       <c r="D32" s="7"/>
@@ -2181,7 +2135,7 @@
         <v>0.72916666666666496</v>
       </c>
       <c r="B33" s="11"/>
-      <c r="C33" s="43"/>
+      <c r="C33" s="32"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
@@ -2192,7 +2146,7 @@
         <v>0.73958333333333104</v>
       </c>
       <c r="B34" s="11"/>
-      <c r="C34" s="43"/>
+      <c r="C34" s="32"/>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
@@ -2203,7 +2157,7 @@
         <v>0.749999999999997</v>
       </c>
       <c r="B35" s="11"/>
-      <c r="C35" s="43"/>
+      <c r="C35" s="32"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
@@ -2214,7 +2168,7 @@
         <v>0.76041666666666297</v>
       </c>
       <c r="B36" s="11"/>
-      <c r="C36" s="43"/>
+      <c r="C36" s="32"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
@@ -2225,7 +2179,7 @@
         <v>0.77083333333332904</v>
       </c>
       <c r="B37" s="11"/>
-      <c r="C37" s="43"/>
+      <c r="C37" s="32"/>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
@@ -2236,7 +2190,7 @@
         <v>0.781249999999996</v>
       </c>
       <c r="B38" s="12"/>
-      <c r="C38" s="44"/>
+      <c r="C38" s="33"/>
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>
       <c r="F38" s="7"/>
@@ -2249,6 +2203,26 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="B3:G6"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="G7:G10"/>
+    <mergeCell ref="G11:G14"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="F11:F14"/>
+    <mergeCell ref="B15:G18"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="C19:C22"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="F19:F22"/>
+    <mergeCell ref="G19:G22"/>
     <mergeCell ref="B32:B38"/>
     <mergeCell ref="C32:C38"/>
     <mergeCell ref="F23:F26"/>
@@ -2263,26 +2237,6 @@
     <mergeCell ref="C23:C26"/>
     <mergeCell ref="D23:D26"/>
     <mergeCell ref="E23:E26"/>
-    <mergeCell ref="B15:G18"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="C19:C22"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="F19:F22"/>
-    <mergeCell ref="G19:G22"/>
-    <mergeCell ref="B3:G6"/>
-    <mergeCell ref="F7:F10"/>
-    <mergeCell ref="G7:G10"/>
-    <mergeCell ref="G11:G14"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="F11:F14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2292,8 +2246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4604F1AA-DEDD-4C2A-B2D1-8301823F4329}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:G38"/>
+    <sheetView zoomScale="105" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2306,11 +2260,11 @@
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="81" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="81" t="s">
         <v>23</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
@@ -2322,68 +2276,68 @@
       <c r="A3" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="19"/>
+      <c r="B3" s="80" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="4">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="22"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="80"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="4">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="22"/>
+      <c r="B5" s="80"/>
+      <c r="C5" s="80"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="80"/>
+      <c r="F5" s="80"/>
+      <c r="G5" s="80"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="4">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B6" s="60"/>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="62"/>
+      <c r="B6" s="80"/>
+      <c r="C6" s="80"/>
+      <c r="D6" s="80"/>
+      <c r="E6" s="80"/>
+      <c r="F6" s="80"/>
+      <c r="G6" s="80"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="56" t="s">
+      <c r="B7" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" s="13" t="s">
+      <c r="D7" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="18" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2391,8 +2345,8 @@
       <c r="A8" s="4">
         <v>0.46875</v>
       </c>
-      <c r="B8" s="57"/>
-      <c r="C8" s="26"/>
+      <c r="B8" s="58"/>
+      <c r="C8" s="22"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
@@ -2402,8 +2356,8 @@
       <c r="A9" s="4">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B9" s="57"/>
-      <c r="C9" s="26"/>
+      <c r="B9" s="58"/>
+      <c r="C9" s="22"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
@@ -2413,8 +2367,8 @@
       <c r="A10" s="4">
         <v>0.48958333333333298</v>
       </c>
-      <c r="B10" s="58"/>
-      <c r="C10" s="59"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="60"/>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
@@ -2424,22 +2378,22 @@
       <c r="A11" s="4">
         <v>0.5</v>
       </c>
-      <c r="B11" s="56" t="s">
+      <c r="B11" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" s="13" t="s">
+      <c r="D11" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="G11" s="18" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2447,8 +2401,8 @@
       <c r="A12" s="4">
         <v>0.51041666666666696</v>
       </c>
-      <c r="B12" s="57"/>
-      <c r="C12" s="26"/>
+      <c r="B12" s="58"/>
+      <c r="C12" s="22"/>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
@@ -2458,8 +2412,8 @@
       <c r="A13" s="4">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B13" s="57"/>
-      <c r="C13" s="26"/>
+      <c r="B13" s="58"/>
+      <c r="C13" s="22"/>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
@@ -2469,8 +2423,8 @@
       <c r="A14" s="4">
         <v>0.53125</v>
       </c>
-      <c r="B14" s="58"/>
-      <c r="C14" s="59"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="60"/>
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
@@ -2480,68 +2434,68 @@
       <c r="A15" s="4">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="63" t="s">
+      <c r="B15" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="32"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="64"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="53"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="4">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="49"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="50"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="38"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="4">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="49"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="50"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="38"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="4">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="65"/>
-      <c r="C18" s="66"/>
-      <c r="D18" s="66"/>
-      <c r="E18" s="66"/>
-      <c r="F18" s="66"/>
-      <c r="G18" s="67"/>
+      <c r="B18" s="54"/>
+      <c r="C18" s="55"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="55"/>
+      <c r="F18" s="55"/>
+      <c r="G18" s="56"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="4">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="56" t="s">
+      <c r="B19" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="E19" s="13" t="s">
+      <c r="D19" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="F19" s="13" t="s">
+      <c r="F19" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="G19" s="13" t="s">
+      <c r="G19" s="18" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2549,8 +2503,8 @@
       <c r="A20" s="4">
         <v>0.59375</v>
       </c>
-      <c r="B20" s="57"/>
-      <c r="C20" s="26"/>
+      <c r="B20" s="58"/>
+      <c r="C20" s="22"/>
       <c r="D20" s="11"/>
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
@@ -2560,8 +2514,8 @@
       <c r="A21" s="4">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B21" s="57"/>
-      <c r="C21" s="26"/>
+      <c r="B21" s="58"/>
+      <c r="C21" s="22"/>
       <c r="D21" s="11"/>
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
@@ -2571,8 +2525,8 @@
       <c r="A22" s="4">
         <v>0.61458333333333304</v>
       </c>
-      <c r="B22" s="58"/>
-      <c r="C22" s="59"/>
+      <c r="B22" s="59"/>
+      <c r="C22" s="60"/>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
@@ -2582,83 +2536,83 @@
       <c r="A23" s="4">
         <v>0.625</v>
       </c>
-      <c r="B23" s="68" t="s">
+      <c r="B23" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E23" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="F23" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="G23" s="13"/>
+      <c r="D23" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="4">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B24" s="69"/>
-      <c r="C24" s="74"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
+      <c r="B24" s="45"/>
+      <c r="C24" s="50"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
       <c r="G24" s="11"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="4">
         <v>0.64583333333333304</v>
       </c>
-      <c r="B25" s="69"/>
-      <c r="C25" s="74"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
+      <c r="B25" s="45"/>
+      <c r="C25" s="50"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
       <c r="G25" s="11"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="4">
         <v>0.65625</v>
       </c>
-      <c r="B26" s="73"/>
-      <c r="C26" s="75"/>
-      <c r="D26" s="37"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
+      <c r="B26" s="49"/>
+      <c r="C26" s="51"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
       <c r="G26" s="12"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="4">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B27" s="68" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" s="39" t="s">
-        <v>22</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="E27" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
+      <c r="B27" s="44" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="4">
         <v>0.67708333333333304</v>
       </c>
-      <c r="B28" s="69"/>
-      <c r="C28" s="71"/>
-      <c r="D28" s="40"/>
-      <c r="E28" s="28"/>
+      <c r="B28" s="45"/>
+      <c r="C28" s="47"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="20"/>
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
     </row>
@@ -2666,10 +2620,10 @@
       <c r="A29" s="4">
         <v>0.6875</v>
       </c>
-      <c r="B29" s="69"/>
-      <c r="C29" s="71"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="28"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="47"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="20"/>
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
     </row>
@@ -2677,10 +2631,10 @@
       <c r="A30" s="4">
         <v>0.69791666666666696</v>
       </c>
-      <c r="B30" s="70"/>
-      <c r="C30" s="72"/>
-      <c r="D30" s="41"/>
-      <c r="E30" s="29"/>
+      <c r="B30" s="46"/>
+      <c r="C30" s="48"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="21"/>
       <c r="F30" s="12"/>
       <c r="G30" s="12"/>
     </row>
@@ -2699,10 +2653,10 @@
       <c r="A32" s="4">
         <v>0.718749999999999</v>
       </c>
-      <c r="B32" s="38" t="s">
+      <c r="B32" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C32" s="38" t="s">
+      <c r="C32" s="13" t="s">
         <v>8</v>
       </c>
       <c r="D32" s="7"/>
@@ -2714,8 +2668,8 @@
       <c r="A33" s="4">
         <v>0.72916666666666496</v>
       </c>
-      <c r="B33" s="54"/>
-      <c r="C33" s="54"/>
+      <c r="B33" s="61"/>
+      <c r="C33" s="61"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
@@ -2725,8 +2679,8 @@
       <c r="A34" s="4">
         <v>0.73958333333333104</v>
       </c>
-      <c r="B34" s="54"/>
-      <c r="C34" s="54"/>
+      <c r="B34" s="61"/>
+      <c r="C34" s="61"/>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
@@ -2736,8 +2690,8 @@
       <c r="A35" s="4">
         <v>0.749999999999997</v>
       </c>
-      <c r="B35" s="54"/>
-      <c r="C35" s="54"/>
+      <c r="B35" s="61"/>
+      <c r="C35" s="61"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
@@ -2747,8 +2701,8 @@
       <c r="A36" s="4">
         <v>0.76041666666666297</v>
       </c>
-      <c r="B36" s="54"/>
-      <c r="C36" s="54"/>
+      <c r="B36" s="61"/>
+      <c r="C36" s="61"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
@@ -2758,8 +2712,8 @@
       <c r="A37" s="4">
         <v>0.77083333333332904</v>
       </c>
-      <c r="B37" s="54"/>
-      <c r="C37" s="54"/>
+      <c r="B37" s="61"/>
+      <c r="C37" s="61"/>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
@@ -2769,8 +2723,8 @@
       <c r="A38" s="4">
         <v>0.781249999999996</v>
       </c>
-      <c r="B38" s="55"/>
-      <c r="C38" s="55"/>
+      <c r="B38" s="62"/>
+      <c r="C38" s="62"/>
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>
       <c r="F38" s="7"/>
@@ -2783,17 +2737,15 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="G23:G26"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="C27:C30"/>
-    <mergeCell ref="D27:D30"/>
-    <mergeCell ref="E27:E30"/>
-    <mergeCell ref="F27:F30"/>
-    <mergeCell ref="G27:G30"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="C23:C26"/>
-    <mergeCell ref="D23:D26"/>
-    <mergeCell ref="E23:E26"/>
+    <mergeCell ref="B32:B38"/>
+    <mergeCell ref="C32:C38"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="F11:F14"/>
+    <mergeCell ref="F23:F26"/>
     <mergeCell ref="B3:G6"/>
     <mergeCell ref="G7:G10"/>
     <mergeCell ref="G11:G14"/>
@@ -2808,15 +2760,17 @@
     <mergeCell ref="C7:C10"/>
     <mergeCell ref="D7:D10"/>
     <mergeCell ref="E7:E10"/>
-    <mergeCell ref="B32:B38"/>
-    <mergeCell ref="C32:C38"/>
-    <mergeCell ref="F7:F10"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="F11:F14"/>
-    <mergeCell ref="F23:F26"/>
+    <mergeCell ref="G23:G26"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="D27:D30"/>
+    <mergeCell ref="E27:E30"/>
+    <mergeCell ref="F27:F30"/>
+    <mergeCell ref="G27:G30"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="D23:D26"/>
+    <mergeCell ref="E23:E26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2826,8 +2780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D66C3A2-B766-4AEA-9D50-70BB9454FECE}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23:C26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2840,11 +2794,11 @@
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="81" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="81" t="s">
         <v>23</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
@@ -2858,68 +2812,68 @@
       <c r="A3" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="19"/>
+      <c r="B3" s="80" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="4">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="22"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="80"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="4">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="22"/>
+      <c r="B5" s="80"/>
+      <c r="C5" s="80"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="80"/>
+      <c r="F5" s="80"/>
+      <c r="G5" s="80"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="4">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="25"/>
+      <c r="B6" s="80"/>
+      <c r="C6" s="80"/>
+      <c r="D6" s="80"/>
+      <c r="E6" s="80"/>
+      <c r="F6" s="80"/>
+      <c r="G6" s="80"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="26" t="s">
-        <v>17</v>
+      <c r="B7" s="22" t="s">
+        <v>16</v>
       </c>
       <c r="C7" s="42" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="36" t="s">
+      <c r="E7" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="36" t="s">
+      <c r="F7" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="36" t="s">
+      <c r="G7" s="29" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2928,7 +2882,7 @@
         <v>0.46875</v>
       </c>
       <c r="B8" s="11"/>
-      <c r="C8" s="40"/>
+      <c r="C8" s="16"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
@@ -2939,7 +2893,7 @@
         <v>0.47916666666666702</v>
       </c>
       <c r="B9" s="11"/>
-      <c r="C9" s="40"/>
+      <c r="C9" s="16"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
@@ -2950,7 +2904,7 @@
         <v>0.48958333333333298</v>
       </c>
       <c r="B10" s="12"/>
-      <c r="C10" s="41"/>
+      <c r="C10" s="17"/>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
@@ -2960,22 +2914,22 @@
       <c r="A11" s="4">
         <v>0.5</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="45" t="s">
-        <v>49</v>
-      </c>
-      <c r="D11" s="13" t="s">
+      <c r="B11" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="G11" s="18" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2984,7 +2938,7 @@
         <v>0.51041666666666696</v>
       </c>
       <c r="B12" s="11"/>
-      <c r="C12" s="40"/>
+      <c r="C12" s="16"/>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
@@ -2995,7 +2949,7 @@
         <v>0.52083333333333304</v>
       </c>
       <c r="B13" s="11"/>
-      <c r="C13" s="40"/>
+      <c r="C13" s="16"/>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
@@ -3006,7 +2960,7 @@
         <v>0.53125</v>
       </c>
       <c r="B14" s="11"/>
-      <c r="C14" s="40"/>
+      <c r="C14" s="16"/>
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
@@ -3016,68 +2970,68 @@
       <c r="A15" s="4">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="46" t="s">
+      <c r="B15" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="47"/>
-      <c r="D15" s="47"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="47"/>
-      <c r="G15" s="48"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="36"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="4">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="49"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="50"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="38"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="4">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="49"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="50"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="38"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="4">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="51"/>
-      <c r="C18" s="52"/>
-      <c r="D18" s="52"/>
-      <c r="E18" s="52"/>
-      <c r="F18" s="52"/>
-      <c r="G18" s="53"/>
+      <c r="B18" s="39"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="41"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="4">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="26" t="s">
-        <v>16</v>
+      <c r="B19" s="22" t="s">
+        <v>15</v>
       </c>
       <c r="C19" s="42" t="s">
-        <v>50</v>
-      </c>
-      <c r="D19" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="E19" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="F19" s="13" t="s">
+      <c r="F19" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="G19" s="13" t="s">
+      <c r="G19" s="18" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3086,7 +3040,7 @@
         <v>0.59375</v>
       </c>
       <c r="B20" s="11"/>
-      <c r="C20" s="40"/>
+      <c r="C20" s="16"/>
       <c r="D20" s="11"/>
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
@@ -3097,7 +3051,7 @@
         <v>0.60416666666666696</v>
       </c>
       <c r="B21" s="11"/>
-      <c r="C21" s="40"/>
+      <c r="C21" s="16"/>
       <c r="D21" s="11"/>
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
@@ -3108,7 +3062,7 @@
         <v>0.61458333333333304</v>
       </c>
       <c r="B22" s="12"/>
-      <c r="C22" s="41"/>
+      <c r="C22" s="17"/>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
@@ -3118,22 +3072,22 @@
       <c r="A23" s="4">
         <v>0.625</v>
       </c>
-      <c r="B23" s="35" t="s">
+      <c r="B23" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E23" s="27" t="s">
+      <c r="D23" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="F23" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="G23" s="13"/>
+      <c r="G23" s="18"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="4">
@@ -3142,8 +3096,8 @@
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
       <c r="D24" s="11"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
       <c r="G24" s="11"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
@@ -3153,8 +3107,8 @@
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
       <c r="D25" s="11"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
       <c r="G25" s="11"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
@@ -3164,37 +3118,37 @@
       <c r="B26" s="12"/>
       <c r="C26" s="12"/>
       <c r="D26" s="12"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
       <c r="G26" s="12"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="4">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B27" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" s="39" t="s">
-        <v>22</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="E27" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
+      <c r="B27" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="4">
         <v>0.67708333333333304</v>
       </c>
       <c r="B28" s="11"/>
-      <c r="C28" s="40"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="28"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="20"/>
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
     </row>
@@ -3203,9 +3157,9 @@
         <v>0.6875</v>
       </c>
       <c r="B29" s="11"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="28"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="20"/>
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
     </row>
@@ -3214,9 +3168,9 @@
         <v>0.69791666666666696</v>
       </c>
       <c r="B30" s="12"/>
-      <c r="C30" s="41"/>
-      <c r="D30" s="37"/>
-      <c r="E30" s="29"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="21"/>
       <c r="F30" s="12"/>
       <c r="G30" s="12"/>
     </row>
@@ -3235,10 +3189,10 @@
       <c r="A32" s="4">
         <v>0.718749999999999</v>
       </c>
-      <c r="B32" s="38" t="s">
+      <c r="B32" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C32" s="38" t="s">
+      <c r="C32" s="13" t="s">
         <v>8</v>
       </c>
       <c r="D32" s="5"/>
@@ -3319,11 +3273,19 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B32:B38"/>
-    <mergeCell ref="C32:C38"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="C27:C30"/>
-    <mergeCell ref="D27:D30"/>
+    <mergeCell ref="G11:G14"/>
+    <mergeCell ref="B3:G6"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="G7:G10"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="F11:F14"/>
     <mergeCell ref="G23:G26"/>
     <mergeCell ref="E27:E30"/>
     <mergeCell ref="B15:G18"/>
@@ -3340,19 +3302,11 @@
     <mergeCell ref="F23:F26"/>
     <mergeCell ref="F27:F30"/>
     <mergeCell ref="G27:G30"/>
-    <mergeCell ref="G11:G14"/>
-    <mergeCell ref="B3:G6"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="F7:F10"/>
-    <mergeCell ref="G7:G10"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="F11:F14"/>
+    <mergeCell ref="B32:B38"/>
+    <mergeCell ref="C32:C38"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="D27:D30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3362,8 +3316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F82DEF69-E5FD-41F0-9622-94C4199D6A7C}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3377,10 +3331,10 @@
         <v>9</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
@@ -3390,232 +3344,232 @@
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="82" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="83"/>
-      <c r="D3" s="83"/>
-      <c r="E3" s="83"/>
-      <c r="F3" s="84"/>
+      <c r="B3" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="4">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="85"/>
-      <c r="C4" s="86"/>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="87"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="4">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="85"/>
-      <c r="C5" s="86"/>
-      <c r="D5" s="86"/>
-      <c r="E5" s="86"/>
-      <c r="F5" s="87"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="4">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B6" s="85"/>
-      <c r="C6" s="86"/>
-      <c r="D6" s="86"/>
-      <c r="E6" s="86"/>
-      <c r="F6" s="87"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="76" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="88"/>
-      <c r="D7" s="88"/>
-      <c r="E7" s="88"/>
-      <c r="F7" s="89"/>
+      <c r="B7" s="63" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="69"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="70"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="4">
         <v>0.46875</v>
       </c>
-      <c r="B8" s="90"/>
-      <c r="C8" s="88"/>
-      <c r="D8" s="88"/>
-      <c r="E8" s="88"/>
-      <c r="F8" s="89"/>
+      <c r="B8" s="71"/>
+      <c r="C8" s="69"/>
+      <c r="D8" s="69"/>
+      <c r="E8" s="69"/>
+      <c r="F8" s="70"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="4">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B9" s="90"/>
-      <c r="C9" s="88"/>
-      <c r="D9" s="88"/>
-      <c r="E9" s="88"/>
-      <c r="F9" s="89"/>
+      <c r="B9" s="71"/>
+      <c r="C9" s="69"/>
+      <c r="D9" s="69"/>
+      <c r="E9" s="69"/>
+      <c r="F9" s="70"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="4">
         <v>0.48958333333333298</v>
       </c>
-      <c r="B10" s="90"/>
-      <c r="C10" s="88"/>
-      <c r="D10" s="88"/>
-      <c r="E10" s="88"/>
-      <c r="F10" s="89"/>
+      <c r="B10" s="71"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="70"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="4">
         <v>0.5</v>
       </c>
-      <c r="B11" s="90"/>
-      <c r="C11" s="88"/>
-      <c r="D11" s="88"/>
-      <c r="E11" s="88"/>
-      <c r="F11" s="89"/>
+      <c r="B11" s="71"/>
+      <c r="C11" s="69"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="69"/>
+      <c r="F11" s="70"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="4">
         <v>0.51041666666666696</v>
       </c>
-      <c r="B12" s="90"/>
-      <c r="C12" s="88"/>
-      <c r="D12" s="88"/>
-      <c r="E12" s="88"/>
-      <c r="F12" s="89"/>
+      <c r="B12" s="71"/>
+      <c r="C12" s="69"/>
+      <c r="D12" s="69"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="70"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="4">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B13" s="90"/>
-      <c r="C13" s="88"/>
-      <c r="D13" s="88"/>
-      <c r="E13" s="88"/>
-      <c r="F13" s="89"/>
+      <c r="B13" s="71"/>
+      <c r="C13" s="69"/>
+      <c r="D13" s="69"/>
+      <c r="E13" s="69"/>
+      <c r="F13" s="70"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="4">
         <v>0.53125</v>
       </c>
-      <c r="B14" s="90"/>
-      <c r="C14" s="88"/>
-      <c r="D14" s="88"/>
-      <c r="E14" s="88"/>
-      <c r="F14" s="89"/>
+      <c r="B14" s="71"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="69"/>
+      <c r="E14" s="69"/>
+      <c r="F14" s="70"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="4">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="49" t="s">
+      <c r="B15" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="50"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="38"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="4">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="49"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="50"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="38"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="4">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="49"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="50"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="38"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="4">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="49"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="50"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="38"/>
     </row>
     <row r="19" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="4">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="76" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" s="77"/>
-      <c r="D19" s="77"/>
-      <c r="E19" s="77"/>
-      <c r="F19" s="78"/>
+      <c r="B19" s="63" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="64"/>
+      <c r="D19" s="64"/>
+      <c r="E19" s="64"/>
+      <c r="F19" s="65"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="4">
         <v>0.59375</v>
       </c>
-      <c r="B20" s="76"/>
-      <c r="C20" s="77"/>
-      <c r="D20" s="77"/>
-      <c r="E20" s="77"/>
-      <c r="F20" s="78"/>
+      <c r="B20" s="63"/>
+      <c r="C20" s="64"/>
+      <c r="D20" s="64"/>
+      <c r="E20" s="64"/>
+      <c r="F20" s="65"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="4">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B21" s="76"/>
-      <c r="C21" s="77"/>
-      <c r="D21" s="77"/>
-      <c r="E21" s="77"/>
-      <c r="F21" s="78"/>
+      <c r="B21" s="63"/>
+      <c r="C21" s="64"/>
+      <c r="D21" s="64"/>
+      <c r="E21" s="64"/>
+      <c r="F21" s="65"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="4">
         <v>0.61458333333333304</v>
       </c>
-      <c r="B22" s="79"/>
-      <c r="C22" s="80"/>
-      <c r="D22" s="80"/>
-      <c r="E22" s="80"/>
-      <c r="F22" s="81"/>
+      <c r="B22" s="66"/>
+      <c r="C22" s="67"/>
+      <c r="D22" s="67"/>
+      <c r="E22" s="67"/>
+      <c r="F22" s="68"/>
     </row>
     <row r="23" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="4">
         <v>0.625</v>
       </c>
-      <c r="B23" s="74" t="s">
+      <c r="B23" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="74" t="s">
-        <v>12</v>
-      </c>
-      <c r="D23" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="E23" s="91" t="s">
+      <c r="D23" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23" s="72" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23" s="72" t="s">
         <v>28</v>
-      </c>
-      <c r="F23" s="91" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
@@ -3624,9 +3578,9 @@
       </c>
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="4">
@@ -3634,9 +3588,9 @@
       </c>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="4">
@@ -3644,36 +3598,36 @@
       </c>
       <c r="B26" s="12"/>
       <c r="C26" s="12"/>
-      <c r="D26" s="41"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
     </row>
     <row r="27" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="4">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B27" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" s="39" t="s">
-        <v>22</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="E27" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="F27" s="13"/>
+      <c r="B27" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="F27" s="18"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="4">
         <v>0.67708333333333304</v>
       </c>
       <c r="B28" s="11"/>
-      <c r="C28" s="40"/>
-      <c r="D28" s="40"/>
-      <c r="E28" s="28"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="20"/>
       <c r="F28" s="11"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
@@ -3681,9 +3635,9 @@
         <v>0.6875</v>
       </c>
       <c r="B29" s="11"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="28"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="20"/>
       <c r="F29" s="11"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
@@ -3691,9 +3645,9 @@
         <v>0.69791666666666696</v>
       </c>
       <c r="B30" s="12"/>
-      <c r="C30" s="41"/>
-      <c r="D30" s="41"/>
-      <c r="E30" s="29"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="21"/>
       <c r="F30" s="12"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
@@ -3710,10 +3664,10 @@
       <c r="A32" s="4">
         <v>0.718749999999999</v>
       </c>
-      <c r="B32" s="38" t="s">
+      <c r="B32" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C32" s="38" t="s">
+      <c r="C32" s="13" t="s">
         <v>8</v>
       </c>
       <c r="D32" s="7"/>
@@ -3724,7 +3678,7 @@
       <c r="A33" s="4">
         <v>0.72916666666666496</v>
       </c>
-      <c r="B33" s="54"/>
+      <c r="B33" s="61"/>
       <c r="C33" s="11"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
@@ -3734,7 +3688,7 @@
       <c r="A34" s="4">
         <v>0.73958333333333104</v>
       </c>
-      <c r="B34" s="54"/>
+      <c r="B34" s="61"/>
       <c r="C34" s="11"/>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
@@ -3744,7 +3698,7 @@
       <c r="A35" s="4">
         <v>0.749999999999997</v>
       </c>
-      <c r="B35" s="54"/>
+      <c r="B35" s="61"/>
       <c r="C35" s="11"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
@@ -3754,7 +3708,7 @@
       <c r="A36" s="4">
         <v>0.76041666666666297</v>
       </c>
-      <c r="B36" s="54"/>
+      <c r="B36" s="61"/>
       <c r="C36" s="11"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
@@ -3764,7 +3718,7 @@
       <c r="A37" s="4">
         <v>0.77083333333332904</v>
       </c>
-      <c r="B37" s="54"/>
+      <c r="B37" s="61"/>
       <c r="C37" s="11"/>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
@@ -3774,7 +3728,7 @@
       <c r="A38" s="4">
         <v>0.781249999999996</v>
       </c>
-      <c r="B38" s="55"/>
+      <c r="B38" s="62"/>
       <c r="C38" s="12"/>
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>
@@ -3786,11 +3740,15 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="20">
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="C3:C6"/>
+    <mergeCell ref="D3:D6"/>
+    <mergeCell ref="E3:E6"/>
+    <mergeCell ref="F3:F6"/>
     <mergeCell ref="B19:F22"/>
     <mergeCell ref="B32:B38"/>
     <mergeCell ref="C32:C38"/>
-    <mergeCell ref="B3:F6"/>
     <mergeCell ref="B7:F14"/>
     <mergeCell ref="B15:F18"/>
     <mergeCell ref="B23:B26"/>
@@ -3831,317 +3789,317 @@
       <c r="A2" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B2" s="92" t="s">
-        <v>32</v>
+      <c r="B2" s="74" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="4">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B3" s="92"/>
+      <c r="B3" s="74"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="4">
         <v>0.4375</v>
       </c>
-      <c r="B4" s="92"/>
+      <c r="B4" s="74"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="4">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B5" s="92"/>
+      <c r="B5" s="74"/>
     </row>
     <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B6" s="93" t="s">
-        <v>33</v>
+      <c r="B6" s="76" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="4">
         <v>0.46875</v>
       </c>
-      <c r="B7" s="93"/>
+      <c r="B7" s="76"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" s="4">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B8" s="93"/>
+      <c r="B8" s="76"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="4">
         <v>0.48958333333333298</v>
       </c>
-      <c r="B9" s="93"/>
+      <c r="B9" s="76"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" s="4">
         <v>0.5</v>
       </c>
-      <c r="B10" s="93"/>
+      <c r="B10" s="76"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" s="4">
         <v>0.51041666666666696</v>
       </c>
-      <c r="B11" s="93"/>
+      <c r="B11" s="76"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" s="4">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B12" s="93"/>
+      <c r="B12" s="76"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" s="4">
         <v>0.53125</v>
       </c>
-      <c r="B13" s="93"/>
+      <c r="B13" s="76"/>
     </row>
     <row r="14" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="4">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B14" s="94" t="s">
-        <v>19</v>
+      <c r="B14" s="77" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="4">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B15" s="95"/>
+      <c r="B15" s="78"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" s="4">
         <v>0.5625</v>
       </c>
-      <c r="B16" s="95"/>
+      <c r="B16" s="78"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" s="4">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B17" s="95"/>
+      <c r="B17" s="78"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" s="4">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B18" s="96"/>
+      <c r="B18" s="79"/>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="4">
         <v>0.59375</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="4">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B20" s="93" t="s">
-        <v>20</v>
+      <c r="B20" s="76" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" s="4">
         <v>0.61458333333333304</v>
       </c>
-      <c r="B21" s="93"/>
+      <c r="B21" s="76"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22" s="4">
         <v>0.625</v>
       </c>
-      <c r="B22" s="93"/>
+      <c r="B22" s="76"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" s="4">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B23" s="93"/>
+      <c r="B23" s="76"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A24" s="4">
         <v>0.64583333333333304</v>
       </c>
-      <c r="B24" s="93"/>
+      <c r="B24" s="76"/>
     </row>
     <row r="25" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="4">
         <v>0.65625</v>
       </c>
-      <c r="B25" s="93"/>
+      <c r="B25" s="76"/>
     </row>
     <row r="26" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="4">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B26" s="93" t="s">
-        <v>21</v>
+      <c r="B26" s="76" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A27" s="4">
         <v>0.67708333333333304</v>
       </c>
-      <c r="B27" s="93"/>
+      <c r="B27" s="76"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A28" s="4">
         <v>0.6875</v>
       </c>
-      <c r="B28" s="93"/>
+      <c r="B28" s="76"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A29" s="4">
         <v>0.69791666666666696</v>
       </c>
-      <c r="B29" s="97" t="s">
-        <v>51</v>
+      <c r="B29" s="73" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A30" s="4">
         <v>0.70833333333333304</v>
       </c>
-      <c r="B30" s="97"/>
+      <c r="B30" s="73"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A31" s="4">
         <v>0.718749999999999</v>
       </c>
-      <c r="B31" s="97"/>
+      <c r="B31" s="73"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A32" s="4">
         <v>0.72916666666666496</v>
       </c>
-      <c r="B32" s="92" t="s">
-        <v>22</v>
+      <c r="B32" s="74" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A33" s="4">
         <v>0.73958333333333104</v>
       </c>
-      <c r="B33" s="92"/>
+      <c r="B33" s="74"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34" s="4">
         <v>0.749999999999997</v>
       </c>
-      <c r="B34" s="92"/>
+      <c r="B34" s="74"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A35" s="4">
         <v>0.76041666666666297</v>
       </c>
-      <c r="B35" s="92"/>
+      <c r="B35" s="74"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A36" s="4">
         <v>0.77083333333332904</v>
       </c>
-      <c r="B36" s="98" t="s">
-        <v>52</v>
+      <c r="B36" s="75" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A37" s="4">
         <v>0.781249999999996</v>
       </c>
-      <c r="B37" s="98"/>
+      <c r="B37" s="75"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A38" s="4">
         <v>0.79166666666666197</v>
       </c>
-      <c r="B38" s="98"/>
+      <c r="B38" s="75"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A39" s="4">
         <v>0.80208333333332804</v>
       </c>
-      <c r="B39" s="98"/>
+      <c r="B39" s="75"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A40" s="4">
         <v>0.812499999999994</v>
       </c>
-      <c r="B40" s="98"/>
+      <c r="B40" s="75"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A41" s="4">
         <v>0.82291666666665997</v>
       </c>
-      <c r="B41" s="92" t="s">
-        <v>53</v>
+      <c r="B41" s="74" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A42" s="4">
         <v>0.83333333333332604</v>
       </c>
-      <c r="B42" s="92"/>
+      <c r="B42" s="74"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A43" s="4">
         <v>0.84374999999999201</v>
       </c>
-      <c r="B43" s="92"/>
+      <c r="B43" s="74"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A44" s="4">
         <v>0.85416666666665797</v>
       </c>
-      <c r="B44" s="97" t="s">
-        <v>54</v>
+      <c r="B44" s="73" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A45" s="4">
         <v>0.86458333333332404</v>
       </c>
-      <c r="B45" s="97"/>
+      <c r="B45" s="73"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A46" s="4">
         <v>0.87499999999999001</v>
       </c>
-      <c r="B46" s="97"/>
+      <c r="B46" s="73"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A47" s="4">
         <v>0.88541666666665597</v>
       </c>
-      <c r="B47" s="97"/>
+      <c r="B47" s="73"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A48" s="4">
         <v>0.89583333333332205</v>
       </c>
-      <c r="B48" s="97"/>
+      <c r="B48" s="73"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A49" s="4">
         <v>0.90624999999998801</v>
       </c>
-      <c r="B49" s="97"/>
+      <c r="B49" s="73"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A50" s="4">
         <v>0.91666666666665497</v>
       </c>
-      <c r="B50" s="97"/>
+      <c r="B50" s="73"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A51" s="4">
@@ -4180,16 +4138,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B6:B13"/>
+    <mergeCell ref="B14:B18"/>
+    <mergeCell ref="B20:B25"/>
+    <mergeCell ref="B26:B28"/>
     <mergeCell ref="B29:B31"/>
     <mergeCell ref="B32:B35"/>
     <mergeCell ref="B36:B40"/>
     <mergeCell ref="B41:B43"/>
     <mergeCell ref="B44:B50"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B6:B13"/>
-    <mergeCell ref="B14:B18"/>
-    <mergeCell ref="B20:B25"/>
-    <mergeCell ref="B26:B28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update student timetable generation to increase row height for time and data rows, enhancing readability. Remove outdated teacher timetable file for the Maritime Museum briefing.
</commit_message>
<xml_diff>
--- a/input/flute-campA-time-table.xlsx
+++ b/input/flute-campA-time-table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lmski\Desktop\Timetable\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lapmi\Desktop\summer-camp-time-table\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56912D3F-5AEB-4A1B-BE96-41FDABAB9A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB8FC01-645C-4079-88CD-B821F252AF9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="503" windowWidth="24196" windowHeight="13875" activeTab="4" xr2:uid="{4F305ACA-9255-4D6C-9A65-1407DE2CF383}"/>
+    <workbookView xWindow="0" yWindow="315" windowWidth="14970" windowHeight="11273" activeTab="5" xr2:uid="{4F305ACA-9255-4D6C-9A65-1407DE2CF383}"/>
   </bookViews>
   <sheets>
     <sheet name="Day 1" sheetId="1" r:id="rId1"/>
@@ -649,92 +649,122 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -743,44 +773,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -801,6 +793,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -813,6 +813,36 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -820,36 +850,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1220,68 +1220,68 @@
       <c r="A3" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="4">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="4">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="4">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
     </row>
     <row r="7" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="28" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1289,55 +1289,55 @@
       <c r="A8" s="4">
         <v>0.46875</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="4">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="4">
         <v>0.48958333333333298</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="4">
         <v>0.5</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="D11" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="G11" s="12" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1345,101 +1345,101 @@
       <c r="A12" s="4">
         <v>0.51041666666666696</v>
       </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="4">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="4">
         <v>0.53125</v>
       </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="4">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="4">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="23"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="4">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="4">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="4">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D19" s="18" t="s">
+      <c r="D19" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="E19" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="F19" s="13" t="s">
+      <c r="F19" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="G19" s="13" t="s">
+      <c r="G19" s="28" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1447,140 +1447,140 @@
       <c r="A20" s="4">
         <v>0.59375</v>
       </c>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="4">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="4">
         <v>0.61458333333333304</v>
       </c>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="4">
         <v>0.625</v>
       </c>
-      <c r="B23" s="25" t="s">
+      <c r="B23" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="25" t="s">
+      <c r="C23" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="22" t="s">
+      <c r="D23" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="E23" s="27" t="s">
+      <c r="E23" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="4">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="4">
         <v>0.64583333333333304</v>
       </c>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="4">
         <v>0.65625</v>
       </c>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="4">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="26" t="s">
+      <c r="C27" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D27" s="22" t="s">
+      <c r="D27" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="E27" s="27" t="s">
+      <c r="E27" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="F27" s="27" t="s">
+      <c r="F27" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="G27" s="16"/>
+      <c r="G27" s="12"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="4">
         <v>0.67708333333333304</v>
       </c>
-      <c r="B28" s="14"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="14"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="13"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="4">
         <v>0.6875</v>
       </c>
-      <c r="B29" s="14"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="28"/>
-      <c r="G29" s="14"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="13"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="4">
         <v>0.69791666666666696</v>
       </c>
-      <c r="B30" s="15"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="29"/>
-      <c r="F30" s="29"/>
-      <c r="G30" s="15"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="14"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="4">
@@ -1593,10 +1593,10 @@
       <c r="A32" s="4">
         <v>0.718749999999999</v>
       </c>
-      <c r="B32" s="24" t="s">
+      <c r="B32" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C32" s="24" t="s">
+      <c r="C32" s="15" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1604,43 +1604,43 @@
       <c r="A33" s="4">
         <v>0.72916666666666496</v>
       </c>
-      <c r="B33" s="14"/>
-      <c r="C33" s="14"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="13"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A34" s="4">
         <v>0.73958333333333104</v>
       </c>
-      <c r="B34" s="14"/>
-      <c r="C34" s="14"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A35" s="4">
         <v>0.749999999999997</v>
       </c>
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A36" s="4">
         <v>0.76041666666666297</v>
       </c>
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="13"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A37" s="4">
         <v>0.77083333333332904</v>
       </c>
-      <c r="B37" s="14"/>
-      <c r="C37" s="14"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A38" s="4">
         <v>0.781249999999996</v>
       </c>
-      <c r="B38" s="15"/>
-      <c r="C38" s="15"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="14"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A39" s="4">
@@ -1649,6 +1649,26 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="B3:G6"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="G7:G10"/>
+    <mergeCell ref="F11:F14"/>
+    <mergeCell ref="G11:G14"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="B15:G18"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="C19:C22"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="F19:F22"/>
+    <mergeCell ref="G19:G22"/>
     <mergeCell ref="F23:F26"/>
     <mergeCell ref="G27:G30"/>
     <mergeCell ref="B32:B38"/>
@@ -1663,26 +1683,6 @@
     <mergeCell ref="B23:B26"/>
     <mergeCell ref="C23:C26"/>
     <mergeCell ref="D23:D26"/>
-    <mergeCell ref="B15:G18"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="C19:C22"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="F19:F22"/>
-    <mergeCell ref="G19:G22"/>
-    <mergeCell ref="B3:G6"/>
-    <mergeCell ref="F7:F10"/>
-    <mergeCell ref="G7:G10"/>
-    <mergeCell ref="F11:F14"/>
-    <mergeCell ref="G11:G14"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="E11:E14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1722,68 +1722,68 @@
       <c r="A3" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="4">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="4">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="4">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="28" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1791,55 +1791,55 @@
       <c r="A8" s="4">
         <v>0.46875</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="4">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="4">
         <v>0.48958333333333298</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="4">
         <v>0.5</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="34" t="s">
+      <c r="C11" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="G11" s="12" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1847,101 +1847,101 @@
       <c r="A12" s="4">
         <v>0.51041666666666696</v>
       </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="4">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="4">
         <v>0.53125</v>
       </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="32"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="4">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="35" t="s">
+      <c r="B15" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="37"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="35"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="4">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="38"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="40"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="38"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="4">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="38"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="40"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="38"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="4">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="41"/>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="43"/>
+      <c r="B18" s="39"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="41"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="4">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="31" t="s">
+      <c r="C19" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="E19" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="F19" s="13" t="s">
+      <c r="F19" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="G19" s="13" t="s">
+      <c r="G19" s="28" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1949,140 +1949,140 @@
       <c r="A20" s="4">
         <v>0.59375</v>
       </c>
-      <c r="B20" s="14"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="4">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B21" s="14"/>
-      <c r="C21" s="32"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="4">
         <v>0.61458333333333304</v>
       </c>
-      <c r="B22" s="15"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
     </row>
     <row r="23" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="4">
         <v>0.625</v>
       </c>
-      <c r="B23" s="25" t="s">
+      <c r="B23" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="25" t="s">
+      <c r="C23" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="22" t="s">
+      <c r="D23" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="E23" s="27" t="s">
+      <c r="E23" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="4">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="4">
         <v>0.64583333333333304</v>
       </c>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="4">
         <v>0.65625</v>
       </c>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
     </row>
     <row r="27" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="4">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="26" t="s">
+      <c r="C27" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D27" s="22" t="s">
+      <c r="D27" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="E27" s="27" t="s">
+      <c r="E27" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="F27" s="27" t="s">
+      <c r="F27" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="G27" s="16"/>
+      <c r="G27" s="12"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="4">
         <v>0.67708333333333304</v>
       </c>
-      <c r="B28" s="14"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="14"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="13"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="4">
         <v>0.6875</v>
       </c>
-      <c r="B29" s="14"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="28"/>
-      <c r="G29" s="14"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="13"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="4">
         <v>0.69791666666666696</v>
       </c>
-      <c r="B30" s="15"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="29"/>
-      <c r="F30" s="29"/>
-      <c r="G30" s="15"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="14"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="4">
@@ -2099,10 +2099,10 @@
       <c r="A32" s="4">
         <v>0.718749999999999</v>
       </c>
-      <c r="B32" s="24" t="s">
+      <c r="B32" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C32" s="24" t="s">
+      <c r="C32" s="15" t="s">
         <v>8</v>
       </c>
       <c r="D32" s="7"/>
@@ -2114,8 +2114,8 @@
       <c r="A33" s="4">
         <v>0.72916666666666496</v>
       </c>
-      <c r="B33" s="14"/>
-      <c r="C33" s="32"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="31"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
@@ -2125,8 +2125,8 @@
       <c r="A34" s="4">
         <v>0.73958333333333104</v>
       </c>
-      <c r="B34" s="14"/>
-      <c r="C34" s="32"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="31"/>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
@@ -2136,8 +2136,8 @@
       <c r="A35" s="4">
         <v>0.749999999999997</v>
       </c>
-      <c r="B35" s="14"/>
-      <c r="C35" s="32"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="31"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
@@ -2147,8 +2147,8 @@
       <c r="A36" s="4">
         <v>0.76041666666666297</v>
       </c>
-      <c r="B36" s="14"/>
-      <c r="C36" s="32"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="31"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
@@ -2158,8 +2158,8 @@
       <c r="A37" s="4">
         <v>0.77083333333332904</v>
       </c>
-      <c r="B37" s="14"/>
-      <c r="C37" s="32"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="31"/>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
@@ -2169,8 +2169,8 @@
       <c r="A38" s="4">
         <v>0.781249999999996</v>
       </c>
-      <c r="B38" s="15"/>
-      <c r="C38" s="33"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="32"/>
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>
       <c r="F38" s="7"/>
@@ -2183,6 +2183,26 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="B3:G6"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="G7:G10"/>
+    <mergeCell ref="G11:G14"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="F11:F14"/>
+    <mergeCell ref="B15:G18"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="C19:C22"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="F19:F22"/>
+    <mergeCell ref="G19:G22"/>
     <mergeCell ref="B32:B38"/>
     <mergeCell ref="C32:C38"/>
     <mergeCell ref="F23:F26"/>
@@ -2197,26 +2217,6 @@
     <mergeCell ref="C23:C26"/>
     <mergeCell ref="D23:D26"/>
     <mergeCell ref="E23:E26"/>
-    <mergeCell ref="B15:G18"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="C19:C22"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="E19:E22"/>
-    <mergeCell ref="F19:F22"/>
-    <mergeCell ref="G19:G22"/>
-    <mergeCell ref="B3:G6"/>
-    <mergeCell ref="F7:F10"/>
-    <mergeCell ref="G7:G10"/>
-    <mergeCell ref="G11:G14"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="F11:F14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2256,68 +2256,68 @@
       <c r="A3" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="4">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="4">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="4">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="22" t="s">
+      <c r="F7" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G7" s="22" t="s">
+      <c r="G7" s="20" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2325,55 +2325,55 @@
       <c r="A8" s="4">
         <v>0.46875</v>
       </c>
-      <c r="B8" s="47"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
+      <c r="B8" s="51"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="4">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B9" s="47"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
+      <c r="B9" s="51"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="4">
         <v>0.48958333333333298</v>
       </c>
-      <c r="B10" s="48"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
+      <c r="B10" s="52"/>
+      <c r="C10" s="53"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="4">
         <v>0.5</v>
       </c>
-      <c r="B11" s="46" t="s">
+      <c r="B11" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="D11" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="22" t="s">
+      <c r="E11" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="22" t="s">
+      <c r="F11" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="G11" s="22" t="s">
+      <c r="G11" s="20" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2381,101 +2381,101 @@
       <c r="A12" s="4">
         <v>0.51041666666666696</v>
       </c>
-      <c r="B12" s="47"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
+      <c r="B12" s="51"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="4">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B13" s="47"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
+      <c r="B13" s="51"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="4">
         <v>0.53125</v>
       </c>
-      <c r="B14" s="48"/>
-      <c r="C14" s="49"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="53"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="4">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="50" t="s">
+      <c r="B15" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="51"/>
-      <c r="D15" s="51"/>
-      <c r="E15" s="51"/>
-      <c r="F15" s="51"/>
-      <c r="G15" s="52"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="46"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="4">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="38"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="40"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="38"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="4">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="38"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="40"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="38"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="4">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="53"/>
-      <c r="C18" s="54"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="54"/>
-      <c r="F18" s="54"/>
-      <c r="G18" s="55"/>
+      <c r="B18" s="47"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="48"/>
+      <c r="G18" s="49"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="4">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="46" t="s">
+      <c r="B19" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="21" t="s">
+      <c r="C19" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="22" t="s">
+      <c r="D19" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="E19" s="22" t="s">
+      <c r="E19" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="F19" s="22" t="s">
+      <c r="F19" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G19" s="22" t="s">
+      <c r="G19" s="20" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2483,140 +2483,140 @@
       <c r="A20" s="4">
         <v>0.59375</v>
       </c>
-      <c r="B20" s="47"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
+      <c r="B20" s="51"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="4">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B21" s="47"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
+      <c r="B21" s="51"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="4">
         <v>0.61458333333333304</v>
       </c>
-      <c r="B22" s="48"/>
-      <c r="C22" s="49"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
+      <c r="B22" s="52"/>
+      <c r="C22" s="53"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
     </row>
     <row r="23" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="4">
         <v>0.625</v>
       </c>
-      <c r="B23" s="25" t="s">
+      <c r="B23" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="25" t="s">
+      <c r="C23" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="22" t="s">
+      <c r="D23" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="E23" s="27" t="s">
+      <c r="E23" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="4">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="4">
         <v>0.64583333333333304</v>
       </c>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="4">
         <v>0.65625</v>
       </c>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
     </row>
     <row r="27" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="4">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="26" t="s">
+      <c r="C27" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D27" s="22" t="s">
+      <c r="D27" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="E27" s="27" t="s">
+      <c r="E27" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="F27" s="27" t="s">
+      <c r="F27" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="G27" s="16"/>
+      <c r="G27" s="12"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="4">
         <v>0.67708333333333304</v>
       </c>
-      <c r="B28" s="14"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="14"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="13"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="4">
         <v>0.6875</v>
       </c>
-      <c r="B29" s="14"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="28"/>
-      <c r="G29" s="14"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="13"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="4">
         <v>0.69791666666666696</v>
       </c>
-      <c r="B30" s="15"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="29"/>
-      <c r="F30" s="29"/>
-      <c r="G30" s="15"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="14"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="4">
@@ -2633,10 +2633,10 @@
       <c r="A32" s="4">
         <v>0.718749999999999</v>
       </c>
-      <c r="B32" s="24" t="s">
+      <c r="B32" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C32" s="24" t="s">
+      <c r="C32" s="15" t="s">
         <v>8</v>
       </c>
       <c r="D32" s="7"/>
@@ -2648,8 +2648,8 @@
       <c r="A33" s="4">
         <v>0.72916666666666496</v>
       </c>
-      <c r="B33" s="44"/>
-      <c r="C33" s="44"/>
+      <c r="B33" s="54"/>
+      <c r="C33" s="54"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
@@ -2659,8 +2659,8 @@
       <c r="A34" s="4">
         <v>0.73958333333333104</v>
       </c>
-      <c r="B34" s="44"/>
-      <c r="C34" s="44"/>
+      <c r="B34" s="54"/>
+      <c r="C34" s="54"/>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
@@ -2670,8 +2670,8 @@
       <c r="A35" s="4">
         <v>0.749999999999997</v>
       </c>
-      <c r="B35" s="44"/>
-      <c r="C35" s="44"/>
+      <c r="B35" s="54"/>
+      <c r="C35" s="54"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
@@ -2681,8 +2681,8 @@
       <c r="A36" s="4">
         <v>0.76041666666666297</v>
       </c>
-      <c r="B36" s="44"/>
-      <c r="C36" s="44"/>
+      <c r="B36" s="54"/>
+      <c r="C36" s="54"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
@@ -2692,8 +2692,8 @@
       <c r="A37" s="4">
         <v>0.77083333333332904</v>
       </c>
-      <c r="B37" s="44"/>
-      <c r="C37" s="44"/>
+      <c r="B37" s="54"/>
+      <c r="C37" s="54"/>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
@@ -2703,8 +2703,8 @@
       <c r="A38" s="4">
         <v>0.781249999999996</v>
       </c>
-      <c r="B38" s="45"/>
-      <c r="C38" s="45"/>
+      <c r="B38" s="55"/>
+      <c r="C38" s="55"/>
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>
       <c r="F38" s="7"/>
@@ -2717,17 +2717,15 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="G23:G26"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="C27:C30"/>
-    <mergeCell ref="D27:D30"/>
-    <mergeCell ref="E27:E30"/>
-    <mergeCell ref="F27:F30"/>
-    <mergeCell ref="G27:G30"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="C23:C26"/>
-    <mergeCell ref="D23:D26"/>
-    <mergeCell ref="E23:E26"/>
+    <mergeCell ref="B32:B38"/>
+    <mergeCell ref="C32:C38"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="F11:F14"/>
+    <mergeCell ref="F23:F26"/>
     <mergeCell ref="B3:G6"/>
     <mergeCell ref="G7:G10"/>
     <mergeCell ref="G11:G14"/>
@@ -2742,15 +2740,17 @@
     <mergeCell ref="C7:C10"/>
     <mergeCell ref="D7:D10"/>
     <mergeCell ref="E7:E10"/>
-    <mergeCell ref="B32:B38"/>
-    <mergeCell ref="C32:C38"/>
-    <mergeCell ref="F7:F10"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="F11:F14"/>
-    <mergeCell ref="F23:F26"/>
+    <mergeCell ref="G23:G26"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="D27:D30"/>
+    <mergeCell ref="E27:E30"/>
+    <mergeCell ref="F27:F30"/>
+    <mergeCell ref="G27:G30"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="D23:D26"/>
+    <mergeCell ref="E23:E26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2792,68 +2792,68 @@
       <c r="A3" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="4">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="4">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="4">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="F7" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="18" t="s">
+      <c r="G7" s="24" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2861,55 +2861,55 @@
       <c r="A8" s="4">
         <v>0.46875</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="4">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="4">
         <v>0.48958333333333298</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="4">
         <v>0.5</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="34" t="s">
+      <c r="C11" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="D11" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="22" t="s">
+      <c r="E11" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="F11" s="22" t="s">
+      <c r="F11" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="22" t="s">
+      <c r="G11" s="20" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2917,101 +2917,101 @@
       <c r="A12" s="4">
         <v>0.51041666666666696</v>
       </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="4">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="4">
         <v>0.53125</v>
       </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="4">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B15" s="35" t="s">
+      <c r="B15" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="37"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="35"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="4">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B16" s="38"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="40"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="38"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="4">
         <v>0.5625</v>
       </c>
-      <c r="B17" s="38"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="40"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="38"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="4">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B18" s="41"/>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="43"/>
+      <c r="B18" s="39"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="41"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="4">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="31" t="s">
+      <c r="C19" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="22" t="s">
+      <c r="D19" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="E19" s="22" t="s">
+      <c r="E19" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="F19" s="22" t="s">
+      <c r="F19" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="G19" s="22" t="s">
+      <c r="G19" s="20" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3019,140 +3019,140 @@
       <c r="A20" s="4">
         <v>0.59375</v>
       </c>
-      <c r="B20" s="14"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="4">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B21" s="14"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="4">
         <v>0.61458333333333304</v>
       </c>
-      <c r="B22" s="15"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
     </row>
     <row r="23" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="4">
         <v>0.625</v>
       </c>
-      <c r="B23" s="25" t="s">
+      <c r="B23" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="25" t="s">
+      <c r="C23" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="22" t="s">
+      <c r="D23" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="E23" s="27" t="s">
+      <c r="E23" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="4">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="4">
         <v>0.64583333333333304</v>
       </c>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="4">
         <v>0.65625</v>
       </c>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
     </row>
     <row r="27" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="4">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="63" t="s">
+      <c r="C27" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="D27" s="66" t="s">
+      <c r="D27" s="62" t="s">
         <v>51</v>
       </c>
-      <c r="E27" s="56" t="s">
+      <c r="E27" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="F27" s="56" t="s">
+      <c r="F27" s="64" t="s">
         <v>49</v>
       </c>
-      <c r="G27" s="58"/>
+      <c r="G27" s="66"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="4">
         <v>0.67708333333333304</v>
       </c>
-      <c r="B28" s="14"/>
-      <c r="C28" s="64"/>
-      <c r="D28" s="67"/>
-      <c r="E28" s="57"/>
-      <c r="F28" s="57"/>
-      <c r="G28" s="59"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="60"/>
+      <c r="D28" s="63"/>
+      <c r="E28" s="65"/>
+      <c r="F28" s="65"/>
+      <c r="G28" s="67"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="4">
         <v>0.6875</v>
       </c>
-      <c r="B29" s="14"/>
-      <c r="C29" s="64"/>
-      <c r="D29" s="67"/>
-      <c r="E29" s="57"/>
-      <c r="F29" s="57"/>
-      <c r="G29" s="59"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="60"/>
+      <c r="D29" s="63"/>
+      <c r="E29" s="65"/>
+      <c r="F29" s="65"/>
+      <c r="G29" s="67"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="4">
         <v>0.69791666666666696</v>
       </c>
-      <c r="B30" s="15"/>
-      <c r="C30" s="65"/>
-      <c r="D30" s="67"/>
-      <c r="E30" s="57"/>
-      <c r="F30" s="57"/>
-      <c r="G30" s="59"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="61"/>
+      <c r="D30" s="63"/>
+      <c r="E30" s="65"/>
+      <c r="F30" s="65"/>
+      <c r="G30" s="67"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="4">
@@ -3169,10 +3169,10 @@
       <c r="A32" s="4">
         <v>0.718749999999999</v>
       </c>
-      <c r="B32" s="24" t="s">
+      <c r="B32" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C32" s="60" t="s">
+      <c r="C32" s="56" t="s">
         <v>8</v>
       </c>
       <c r="D32" s="2"/>
@@ -3184,8 +3184,8 @@
       <c r="A33" s="4">
         <v>0.72916666666666496</v>
       </c>
-      <c r="B33" s="14"/>
-      <c r="C33" s="61"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="57"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
@@ -3195,8 +3195,8 @@
       <c r="A34" s="4">
         <v>0.73958333333333104</v>
       </c>
-      <c r="B34" s="14"/>
-      <c r="C34" s="61"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="57"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
@@ -3206,8 +3206,8 @@
       <c r="A35" s="4">
         <v>0.749999999999997</v>
       </c>
-      <c r="B35" s="14"/>
-      <c r="C35" s="61"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="57"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
@@ -3217,8 +3217,8 @@
       <c r="A36" s="4">
         <v>0.76041666666666297</v>
       </c>
-      <c r="B36" s="14"/>
-      <c r="C36" s="61"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="57"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
@@ -3228,8 +3228,8 @@
       <c r="A37" s="4">
         <v>0.77083333333332904</v>
       </c>
-      <c r="B37" s="14"/>
-      <c r="C37" s="61"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="57"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
@@ -3239,8 +3239,8 @@
       <c r="A38" s="4">
         <v>0.781249999999996</v>
       </c>
-      <c r="B38" s="15"/>
-      <c r="C38" s="62"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="58"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
@@ -3253,11 +3253,19 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B32:B38"/>
-    <mergeCell ref="C32:C38"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="C27:C30"/>
-    <mergeCell ref="D27:D30"/>
+    <mergeCell ref="G11:G14"/>
+    <mergeCell ref="B3:G6"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="G7:G10"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="D11:D14"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="F11:F14"/>
     <mergeCell ref="G23:G26"/>
     <mergeCell ref="E27:E30"/>
     <mergeCell ref="B15:G18"/>
@@ -3274,19 +3282,11 @@
     <mergeCell ref="F23:F26"/>
     <mergeCell ref="F27:F30"/>
     <mergeCell ref="G27:G30"/>
-    <mergeCell ref="G11:G14"/>
-    <mergeCell ref="B3:G6"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="F7:F10"/>
-    <mergeCell ref="G7:G10"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="D11:D14"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="F11:F14"/>
+    <mergeCell ref="B32:B38"/>
+    <mergeCell ref="C32:C38"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="D27:D30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3296,7 +3296,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F82DEF69-E5FD-41F0-9622-94C4199D6A7C}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="63" workbookViewId="0">
+    <sheetView zoomScale="63" workbookViewId="0">
       <selection activeCell="B3" sqref="B3:F6"/>
     </sheetView>
   </sheetViews>
@@ -3328,43 +3328,43 @@
       <c r="A3" s="4">
         <v>0.41666666666666669</v>
       </c>
-      <c r="B3" s="76" t="s">
+      <c r="B3" s="72" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="77"/>
-      <c r="D3" s="77"/>
-      <c r="E3" s="77"/>
-      <c r="F3" s="78"/>
+      <c r="C3" s="73"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="74"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="4">
         <v>0.42708333333333331</v>
       </c>
-      <c r="B4" s="79"/>
-      <c r="C4" s="80"/>
-      <c r="D4" s="80"/>
-      <c r="E4" s="80"/>
-      <c r="F4" s="81"/>
+      <c r="B4" s="75"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="77"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="4">
         <v>0.4375</v>
       </c>
-      <c r="B5" s="79"/>
-      <c r="C5" s="80"/>
-      <c r="D5" s="80"/>
-      <c r="E5" s="80"/>
-      <c r="F5" s="81"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="76"/>
+      <c r="D5" s="76"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="77"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="4">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B6" s="82"/>
-      <c r="C6" s="83"/>
-      <c r="D6" s="83"/>
-      <c r="E6" s="83"/>
-      <c r="F6" s="84"/>
+      <c r="B6" s="78"/>
+      <c r="C6" s="79"/>
+      <c r="D6" s="79"/>
+      <c r="E6" s="79"/>
+      <c r="F6" s="80"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="4">
@@ -3542,61 +3542,61 @@
       <c r="C23" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="18" t="s">
+      <c r="D23" s="24" t="s">
         <v>53</v>
       </c>
       <c r="E23" s="71" t="s">
         <v>27</v>
       </c>
-      <c r="F23" s="13"/>
+      <c r="F23" s="28"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="4">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="14"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="13"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="4">
         <v>0.64583333333333304</v>
       </c>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="14"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="13"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="4">
         <v>0.65625</v>
       </c>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="15"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="14"/>
     </row>
     <row r="27" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="4">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="26" t="s">
+      <c r="C27" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D27" s="22" t="s">
+      <c r="D27" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="E27" s="27" t="s">
+      <c r="E27" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="F27" s="27" t="s">
+      <c r="F27" s="21" t="s">
         <v>49</v>
       </c>
     </row>
@@ -3604,31 +3604,31 @@
       <c r="A28" s="4">
         <v>0.67708333333333304</v>
       </c>
-      <c r="B28" s="14"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="4">
         <v>0.6875</v>
       </c>
-      <c r="B29" s="14"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="28"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="4">
         <v>0.69791666666666696</v>
       </c>
-      <c r="B30" s="15"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="29"/>
-      <c r="F30" s="29"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="4">
@@ -3644,10 +3644,10 @@
       <c r="A32" s="4">
         <v>0.718749999999999</v>
       </c>
-      <c r="B32" s="24" t="s">
+      <c r="B32" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C32" s="24" t="s">
+      <c r="C32" s="15" t="s">
         <v>8</v>
       </c>
       <c r="D32" s="7"/>
@@ -3658,8 +3658,8 @@
       <c r="A33" s="4">
         <v>0.72916666666666496</v>
       </c>
-      <c r="B33" s="44"/>
-      <c r="C33" s="14"/>
+      <c r="B33" s="54"/>
+      <c r="C33" s="13"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
@@ -3668,8 +3668,8 @@
       <c r="A34" s="4">
         <v>0.73958333333333104</v>
       </c>
-      <c r="B34" s="44"/>
-      <c r="C34" s="14"/>
+      <c r="B34" s="54"/>
+      <c r="C34" s="13"/>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
@@ -3678,8 +3678,8 @@
       <c r="A35" s="4">
         <v>0.749999999999997</v>
       </c>
-      <c r="B35" s="44"/>
-      <c r="C35" s="14"/>
+      <c r="B35" s="54"/>
+      <c r="C35" s="13"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
@@ -3688,8 +3688,8 @@
       <c r="A36" s="4">
         <v>0.76041666666666297</v>
       </c>
-      <c r="B36" s="44"/>
-      <c r="C36" s="14"/>
+      <c r="B36" s="54"/>
+      <c r="C36" s="13"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
@@ -3698,8 +3698,8 @@
       <c r="A37" s="4">
         <v>0.77083333333332904</v>
       </c>
-      <c r="B37" s="44"/>
-      <c r="C37" s="14"/>
+      <c r="B37" s="54"/>
+      <c r="C37" s="13"/>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
@@ -3708,8 +3708,8 @@
       <c r="A38" s="4">
         <v>0.781249999999996</v>
       </c>
-      <c r="B38" s="45"/>
-      <c r="C38" s="15"/>
+      <c r="B38" s="55"/>
+      <c r="C38" s="14"/>
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>
       <c r="F38" s="7"/>
@@ -3721,6 +3721,7 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B3:F6"/>
     <mergeCell ref="B19:F22"/>
     <mergeCell ref="B32:B38"/>
     <mergeCell ref="C32:C38"/>
@@ -3736,7 +3737,6 @@
     <mergeCell ref="D27:D30"/>
     <mergeCell ref="E27:E30"/>
     <mergeCell ref="F27:F30"/>
-    <mergeCell ref="B3:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3746,8 +3746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F258A27A-E0BD-410A-AC93-E998D70178A7}">
   <dimension ref="A1:B57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51:A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3791,7 +3791,7 @@
       <c r="A6" s="4">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B6" s="66" t="s">
+      <c r="B6" s="62" t="s">
         <v>31</v>
       </c>
     </row>
@@ -3799,49 +3799,49 @@
       <c r="A7" s="4">
         <v>0.46875</v>
       </c>
-      <c r="B7" s="66"/>
+      <c r="B7" s="62"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" s="4">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B8" s="66"/>
+      <c r="B8" s="62"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="4">
         <v>0.48958333333333298</v>
       </c>
-      <c r="B9" s="66"/>
+      <c r="B9" s="62"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" s="4">
         <v>0.5</v>
       </c>
-      <c r="B10" s="66"/>
+      <c r="B10" s="62"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" s="4">
         <v>0.51041666666666696</v>
       </c>
-      <c r="B11" s="66"/>
+      <c r="B11" s="62"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" s="4">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B12" s="66"/>
+      <c r="B12" s="62"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" s="4">
         <v>0.53125</v>
       </c>
-      <c r="B13" s="66"/>
+      <c r="B13" s="62"/>
     </row>
     <row r="14" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="4">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B14" s="72" t="s">
+      <c r="B14" s="82" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3849,25 +3849,25 @@
       <c r="A15" s="4">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B15" s="73"/>
+      <c r="B15" s="83"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" s="4">
         <v>0.5625</v>
       </c>
-      <c r="B16" s="73"/>
+      <c r="B16" s="83"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" s="4">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B17" s="73"/>
+      <c r="B17" s="83"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" s="4">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B18" s="74"/>
+      <c r="B18" s="84"/>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="4">
@@ -3881,7 +3881,7 @@
       <c r="A20" s="4">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B20" s="66" t="s">
+      <c r="B20" s="62" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3889,37 +3889,37 @@
       <c r="A21" s="4">
         <v>0.61458333333333304</v>
       </c>
-      <c r="B21" s="66"/>
+      <c r="B21" s="62"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22" s="4">
         <v>0.625</v>
       </c>
-      <c r="B22" s="66"/>
+      <c r="B22" s="62"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" s="4">
         <v>0.63541666666666696</v>
       </c>
-      <c r="B23" s="66"/>
+      <c r="B23" s="62"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A24" s="4">
         <v>0.64583333333333304</v>
       </c>
-      <c r="B24" s="66"/>
+      <c r="B24" s="62"/>
     </row>
     <row r="25" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="4">
         <v>0.65625</v>
       </c>
-      <c r="B25" s="66"/>
+      <c r="B25" s="62"/>
     </row>
     <row r="26" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="4">
         <v>0.66666666666666696</v>
       </c>
-      <c r="B26" s="66" t="s">
+      <c r="B26" s="62" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3927,19 +3927,19 @@
       <c r="A27" s="4">
         <v>0.67708333333333304</v>
       </c>
-      <c r="B27" s="66"/>
+      <c r="B27" s="62"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A28" s="4">
         <v>0.6875</v>
       </c>
-      <c r="B28" s="66"/>
+      <c r="B28" s="62"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A29" s="4">
         <v>0.69791666666666696</v>
       </c>
-      <c r="B29" s="75" t="s">
+      <c r="B29" s="81" t="s">
         <v>43</v>
       </c>
     </row>
@@ -3947,13 +3947,13 @@
       <c r="A30" s="4">
         <v>0.70833333333333304</v>
       </c>
-      <c r="B30" s="75"/>
+      <c r="B30" s="81"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A31" s="4">
         <v>0.718749999999999</v>
       </c>
-      <c r="B31" s="75"/>
+      <c r="B31" s="81"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A32" s="4">
@@ -4037,7 +4037,7 @@
       <c r="A44" s="4">
         <v>0.85416666666665797</v>
       </c>
-      <c r="B44" s="75" t="s">
+      <c r="B44" s="81" t="s">
         <v>46</v>
       </c>
     </row>
@@ -4045,85 +4045,71 @@
       <c r="A45" s="4">
         <v>0.86458333333332404</v>
       </c>
-      <c r="B45" s="75"/>
+      <c r="B45" s="81"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A46" s="4">
         <v>0.87499999999999001</v>
       </c>
-      <c r="B46" s="75"/>
+      <c r="B46" s="81"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A47" s="4">
         <v>0.88541666666665597</v>
       </c>
-      <c r="B47" s="75"/>
+      <c r="B47" s="81"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A48" s="4">
         <v>0.89583333333332205</v>
       </c>
-      <c r="B48" s="75"/>
+      <c r="B48" s="81"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A49" s="4">
         <v>0.90624999999998801</v>
       </c>
-      <c r="B49" s="75"/>
+      <c r="B49" s="81"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A50" s="4">
         <v>0.91666666666665497</v>
       </c>
-      <c r="B50" s="75"/>
+      <c r="B50" s="81"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A51" s="4">
-        <v>0.92708333333332105</v>
-      </c>
+      <c r="A51" s="4"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A52" s="4">
-        <v>0.93749999999998701</v>
-      </c>
+      <c r="A52" s="4"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A53" s="4">
-        <v>0.94791666666665297</v>
-      </c>
+      <c r="A53" s="4"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A54" s="4">
-        <v>0.95833333333331905</v>
-      </c>
+      <c r="A54" s="4"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A55" s="4">
-        <v>0.96874999999998501</v>
-      </c>
+      <c r="A55" s="4"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A56" s="4">
-        <v>0.97916666666665098</v>
-      </c>
+      <c r="A56" s="4"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A57" s="4">
-        <v>0.98958333333331705</v>
-      </c>
+      <c r="A57" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B6:B13"/>
+    <mergeCell ref="B14:B18"/>
+    <mergeCell ref="B20:B25"/>
+    <mergeCell ref="B26:B28"/>
     <mergeCell ref="B29:B31"/>
     <mergeCell ref="B32:B35"/>
     <mergeCell ref="B36:B40"/>
     <mergeCell ref="B41:B43"/>
     <mergeCell ref="B44:B50"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B6:B13"/>
-    <mergeCell ref="B14:B18"/>
-    <mergeCell ref="B20:B25"/>
-    <mergeCell ref="B26:B28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>